<commit_message>
Updates on 2nd set of images
Updated Excel with second set of images items, renamed the product titles matching product images, added second images (skuxxx_1).
</commit_message>
<xml_diff>
--- a/assets/muproducts.xlsx
+++ b/assets/muproducts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sumi/Dropbox/Employers/ORACLE/PROJECTS/SOCK and MU SHOP/MuShop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A5187F-DF69-D64F-AFFA-B1C676D92BFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2566058-8B00-2F45-958D-904550092E94}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="860" windowWidth="37220" windowHeight="21540" activeTab="1" xr2:uid="{F62C75C7-879A-AF4E-9C80-D3B46F05DAE7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16920" activeTab="1" xr2:uid="{F62C75C7-879A-AF4E-9C80-D3B46F05DAE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -109,9 +109,6 @@
     <t>Litter Accessories</t>
   </si>
   <si>
-    <t>Original Unscented Formula Cat Litter</t>
-  </si>
-  <si>
     <t>SKU</t>
   </si>
   <si>
@@ -229,9 +226,6 @@
     <t>MU-US-027</t>
   </si>
   <si>
-    <t>Instant Action Litter for Multiple Cats</t>
-  </si>
-  <si>
     <t>Tidy Cats</t>
   </si>
   <si>
@@ -244,9 +238,6 @@
     <t>20lbs</t>
   </si>
   <si>
-    <t>Cat Litter Deodorizer</t>
-  </si>
-  <si>
     <t>Choco Spring</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>26Oz</t>
   </si>
   <si>
-    <t>Cat Litter Deodorizer Powder</t>
-  </si>
-  <si>
     <t>20Oz</t>
   </si>
   <si>
@@ -268,9 +256,6 @@
     <t>Arm &amp; Hammer</t>
   </si>
   <si>
-    <t>Cat Litter Pan With Rim</t>
-  </si>
-  <si>
     <t>Petmate</t>
   </si>
   <si>
@@ -283,15 +268,9 @@
     <t>18.7" x 15.5" x 10.6"</t>
   </si>
   <si>
-    <t>Tidy Cat Breeze Cat Litter System</t>
-  </si>
-  <si>
     <t>Change the way you think about cleaning your cat's litter box with the Purina Tidy Cats BREEZE With Ammonia Blocker Litter System starter kit. This system features powerful odor control to keep your house smelling fresh and clean, and the specially designed, cat-friendly litter pellets minimize your pets from tracking litter throughout your home.</t>
   </si>
   <si>
-    <t>Original Pet Fountain</t>
-  </si>
-  <si>
     <t>Petsafe</t>
   </si>
   <si>
@@ -319,9 +298,6 @@
     <t>07</t>
   </si>
   <si>
-    <t>Drinkwell Pagoda Fountain</t>
-  </si>
-  <si>
     <t>The Pagoda fountain continuously recirculates 70 ounces of fresh, filtered water. Best of all, the stylish ceramic design is easy to clean and looks great in your home. The upper and lower dishes provide two drinking areas for pets, and the patented dual free-falling streams aerate the water for freshness, which encourages your pet to drink more.</t>
   </si>
   <si>
@@ -329,9 +305,6 @@
   </si>
   <si>
     <t>red, white</t>
-  </si>
-  <si>
-    <t>Crock Small Animal Bowl</t>
   </si>
   <si>
     <t>08</t>
@@ -345,9 +318,6 @@
   </si>
   <si>
     <t>3"</t>
-  </si>
-  <si>
-    <t>Cat Bella Bowl</t>
   </si>
   <si>
     <t>10</t>
@@ -371,16 +341,9 @@
     <t>11</t>
   </si>
   <si>
-    <t>Meow Placemat</t>
-  </si>
-  <si>
     <t>Petrageous Designs pet placemats are the perfect way to keep your pets' feeding area clean and classy! This ultra-durable Food/Water Placemat keeps nasty spills and stray kibble off your clean floors, while adding playful character to your home's decor. Easy to clean.</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Meow Meow  Bowl Mat</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -390,18 +353,12 @@
     <t>13</t>
   </si>
   <si>
-    <t>Food Storage Container</t>
-  </si>
-  <si>
     <t>Pet Food Storage Container features a tight seal to ensure your pet's food will stay fresh longer, reducing spoilage due to pests and moisture. Made from FDS food contact approved plastic.</t>
   </si>
   <si>
     <t>14</t>
   </si>
   <si>
-    <t>Chicken &amp; Pomegranate Dry Cat Food</t>
-  </si>
-  <si>
     <t>Pet Food</t>
   </si>
   <si>
@@ -414,9 +371,6 @@
     <t>15</t>
   </si>
   <si>
-    <t>Cat and Kitten Grain Free Dry Cat Food</t>
-  </si>
-  <si>
     <t>Cat and Kitten recipe is a grain-free, region-inspired formula that your cat will thrive on. An excellent choice for cats of all breed and ages, this biologically appropriate recipe contains an unmatched variety of fresh regional ingredients delivered daily from local Kentucky farms. Packed with over 75% meat, the recipe features free-fun Cobb chicken, nest-laid eggs, Tom turkey, Blue catfish and Rainbow trout in wholeprey ratios in order to mimic the diet mother nature intended.</t>
   </si>
   <si>
@@ -438,9 +392,6 @@
     <t>Weruva</t>
   </si>
   <si>
-    <t xml:space="preserve">Love Me Tender Pouches </t>
-  </si>
-  <si>
     <t>17</t>
   </si>
   <si>
@@ -462,16 +413,10 @@
     <t>Whether this is your cat’s first urinary issue or they need ongoing urinary care, your vet recommended Royal Canin Urinary SO for a reason. This veterinary-exclusive dry cat food was developed to nutritionally support your adult cat’s urinary tract and bladder health. It increases the amount of urine your cat produces to help dilute excess minerals that can cause crystals and stones.</t>
   </si>
   <si>
-    <t>Care with Chicken Dry Cat Food</t>
-  </si>
-  <si>
     <t xml:space="preserve">A healthy bladder starts with the right balance of vital nutrients. Excess minerals can encourage the formation of crystals in the urine, which may lead to the creation of bladder stones. They can cause discomfort and lead to more serious problems that require the care of a veterinarian. </t>
   </si>
   <si>
     <t>20</t>
-  </si>
-  <si>
-    <t>Wet Canned Cat Food</t>
   </si>
   <si>
     <t>Wellness</t>
@@ -491,9 +436,6 @@
     <t>21</t>
   </si>
   <si>
-    <t>Green Pea Formula Canned Cat Food</t>
-  </si>
-  <si>
     <t>Designed with a limited number of premium protein and carbohydrate sources, this Grain-free cat food is an excellent choice when seeking alternative ingredients for your cat. Natural Balance L.I.D. Limited Ingredient Diets Duck and Green Pea Formula Canned Cat Food is designed to support healthy digestion and to maintain skin and coat health—all while providing complete, balanced nutrition for all life stages!</t>
   </si>
   <si>
@@ -507,18 +449,12 @@
     <t>23</t>
   </si>
   <si>
-    <t>Wire Cat Brush</t>
-  </si>
-  <si>
     <t>Amazing Paw</t>
   </si>
   <si>
     <t>For a well groomed appearance, cats and kittens need to be brushed regularly. The Magic Coat® Slicker Wire Brushes are designed to easily remove mats while pulling out dead hair. Brushing helps stimulate the skin to promote healthy circulation and increase shine.</t>
   </si>
   <si>
-    <t>Groom Genie Cat Brush</t>
-  </si>
-  <si>
     <t>The Groom Genie evolved from a brush designed for humans – the Knot Genie. Rikki Mor, a mom of three, was frustrated with the huge cost and lack of effectiveness of other detangling brushes on the market. So she took matters into her own hands and invented what is now known as The World's Best Detangling Brush.</t>
   </si>
   <si>
@@ -528,9 +464,6 @@
     <t>24</t>
   </si>
   <si>
-    <t>Oatmeal and Aloe Shampoo</t>
-  </si>
-  <si>
     <t>Earthbath specially formulated this Oatmeal &amp; Aloe itch relief shampoo to address the needs of beloved pets with dry, itchy skin. Oatmeal and aloe vera are recommended by veterinarians to effectively combat skin irritation, promote healing, and re-moisturize sensitive, dry skin.</t>
   </si>
   <si>
@@ -540,109 +473,201 @@
     <t>25</t>
   </si>
   <si>
-    <t>Oatmeal and Aloe Conditioner</t>
-  </si>
-  <si>
-    <t>The addition of 3% colloidal oatmeal and aloe vera helps re-moisturize and soothe skin, too. Our sumptuous conditioner will leave your best friend’s coat soft and plush while bringing out its natural luster and brilliance.</t>
-  </si>
-  <si>
     <t>26</t>
   </si>
   <si>
-    <t>Grooming Mitt for Cats</t>
-  </si>
-  <si>
     <t>Cleans and softens cat’s coat, removes loose hair and gently massages. Made with lightweight neoprene material with adjustable closer and soft rubber nubs, the Love Glove® mitt is also great for removing loose cat hair from furniture and clothing.</t>
   </si>
   <si>
     <t>27</t>
   </si>
   <si>
-    <t>Motion Lithium Ion Clipper</t>
-  </si>
-  <si>
     <t xml:space="preserve">Powerful motor up to 5,500 SPM's with integrated rapid power. The '5 in 1' Pro Blade for less breakage and optimal usage. Blade and clipper are ALWAYS cool running. Lithium Ion battery technology gives optimal performance. 90 minutes of cordless runtime with 45 minute quick full charge. Higher performance, longer usage times and consistent reliability. </t>
   </si>
   <si>
-    <t>./products/MU-US-001.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-002.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-003.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-005.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-006.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-004.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-007.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-008.png</t>
-  </si>
-  <si>
     <t>./products/MU-US-009.png</t>
   </si>
   <si>
-    <t>./products/MU-US-013.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-010.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-011.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-012.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-014.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-015.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-018.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-016.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-017.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-019.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-020.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-021.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-022.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-023.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-024.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-025.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-026.png</t>
-  </si>
-  <si>
-    <t>./products/MU-US-027.png</t>
+    <t>./products/MU-US-001.png,
+./products/MU-US-001_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-002.png,
+./products/MU-US-002_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-003.png,
+./products/MU-US-003_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-004.png,
+./products/MU-US-004_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-005.png,
+./products/MU-US-005_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-006.png,
+./products/MU-US-006_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-007.png,
+./products/MU-US-007_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-008.png,
+./products/MU-US-008_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-010.png,
+./products/MU-US-010_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-011.png,
+./products/MU-US-011_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-012.png,
+./products/MU-US-012_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-013.png,
+./products/MU-US-013_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-014.png,
+./products/MU-US-014_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-015.png,
+./products/MU-US-015_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-016.png,
+./products/MU-US-016_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-017.png,
+./products/MU-US-017_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-018.png,
+./products/MU-US-018_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-019.png,
+./products/MU-US-019_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-020.png,
+./products/MU-US-020_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-021.png,
+./products/MU-US-021_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-022.png,
+./products/MU-US-022_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-023.png,
+./products/MU-US-023_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-024.png,
+./products/MU-US-024_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-025.png,
+./products/MU-US-025_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-026.png,
+./products/MU-US-026_1.png</t>
+  </si>
+  <si>
+    <t>./products/MU-US-027.png,
+./products/MU-US-027_1.png</t>
+  </si>
+  <si>
+    <t>Original Unscented Litter Trapper</t>
+  </si>
+  <si>
+    <t>Instant Action Mu BroomKit</t>
+  </si>
+  <si>
+    <t>Mu DeoSpray Deodorizer</t>
+  </si>
+  <si>
+    <t>Mu O-DeoSpray Deodorizer</t>
+  </si>
+  <si>
+    <t>Cat Litter Mu LitterBox</t>
+  </si>
+  <si>
+    <t>Mu X-DeoSpray Deodorizer</t>
+  </si>
+  <si>
+    <t>Original MuMate Bowl</t>
+  </si>
+  <si>
+    <t>Drinkwell BrandX Feeder</t>
+  </si>
+  <si>
+    <t>Crock Small Coastal FishBowl</t>
+  </si>
+  <si>
+    <t>Mu Fusion Bowl</t>
+  </si>
+  <si>
+    <t>Mu Mat Green Placemat</t>
+  </si>
+  <si>
+    <t>Mu Mat Blue Placemat</t>
+  </si>
+  <si>
+    <t>Mu Storage Container</t>
+  </si>
+  <si>
+    <t>Chicken &amp; Pomegranate Mu Cat Food</t>
+  </si>
+  <si>
+    <t>Cat and Kitten BlueHill MagiK</t>
+  </si>
+  <si>
+    <t>Love Me Variety Pack Green</t>
+  </si>
+  <si>
+    <t>Care with Chicken BlueHill MagiK</t>
+  </si>
+  <si>
+    <t>Wet Canned Mu Dry Food</t>
+  </si>
+  <si>
+    <t>Green Pea Formula Mu Cat Food</t>
+  </si>
+  <si>
+    <t>Wire Cat KittyBrush</t>
+  </si>
+  <si>
+    <t>Groom Genie KittyBrush</t>
+  </si>
+  <si>
+    <t>Oatmeal and Aloe 2-in-1 Shampoo</t>
+  </si>
+  <si>
+    <t>Oatmeal and Aloe Protein Shampoo</t>
+  </si>
+  <si>
+    <t>The addition of 3% colloidal oatmeal and aloe vera helps re-moisturize and soothe skin, too. Our sumptuous Shampoo will leave your best friend’s coat soft and plush while bringing out its natural luster and brilliance.</t>
+  </si>
+  <si>
+    <t>GrooMe Kit</t>
+  </si>
+  <si>
+    <t>Motion Lithium Ear Groomer</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1247,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>16</v>
@@ -1258,8 +1283,8 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="I26" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1281,63 +1306,63 @@
   <sheetData>
     <row r="1" spans="1:12" ht="23" customHeight="1">
       <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="70">
       <c r="A2" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F2" s="13" t="s">
         <v>26</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="13">
         <v>0</v>
@@ -1352,30 +1377,30 @@
         <v>18.5</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>176</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="70">
       <c r="A3" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>68</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>70</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H3" s="13">
         <v>0</v>
@@ -1390,30 +1415,30 @@
         <v>28.99</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>177</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="70">
       <c r="A4" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>72</v>
+        <v>179</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H4" s="13">
         <v>0</v>
@@ -1428,30 +1453,30 @@
         <v>7.99</v>
       </c>
       <c r="L4" s="15" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="42">
       <c r="A5" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>76</v>
+        <v>180</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="H5" s="13">
         <v>0</v>
@@ -1466,24 +1491,24 @@
         <v>4.99</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="42">
       <c r="A6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>23</v>
@@ -1492,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I6" s="13">
         <v>0</v>
@@ -1504,24 +1529,24 @@
         <v>9.5</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>179</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="98">
       <c r="A7" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F7" s="13" t="s">
         <v>23</v>
@@ -1530,7 +1555,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="I7" s="13">
         <v>0</v>
@@ -1542,24 +1567,24 @@
         <v>39.25</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>180</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="70">
       <c r="A8" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>87</v>
+        <v>183</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>5</v>
@@ -1580,24 +1605,24 @@
         <v>43.95</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="84">
       <c r="A9" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>97</v>
+        <v>184</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>5</v>
@@ -1609,7 +1634,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="J9" s="13">
         <v>99</v>
@@ -1618,24 +1643,24 @@
         <v>79.95</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="42">
       <c r="A10" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>101</v>
+        <v>185</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>6</v>
@@ -1644,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="I10" s="13">
         <v>0</v>
@@ -1656,24 +1681,24 @@
         <v>4.75</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="98">
       <c r="A11" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>106</v>
+        <v>186</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>6</v>
@@ -1682,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="I11" s="13">
         <v>0</v>
@@ -1691,27 +1716,27 @@
         <v>99</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="70">
       <c r="A12" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>8</v>
@@ -1732,24 +1757,24 @@
         <v>4.99</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="84">
       <c r="A13" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>115</v>
+        <v>98</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>188</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>8</v>
@@ -1770,30 +1795,30 @@
         <v>11.95</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>188</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="56">
       <c r="A14" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>119</v>
+        <v>189</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>9</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14" s="13">
         <v>0</v>
@@ -1808,30 +1833,30 @@
         <v>9.99</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="70">
       <c r="A15" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>122</v>
+        <v>190</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="H15" s="13">
         <v>0</v>
@@ -1846,30 +1871,30 @@
         <v>38.950000000000003</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="126">
       <c r="A16" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>127</v>
+        <v>191</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>10</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="H16" s="13">
         <v>0</v>
@@ -1884,30 +1909,30 @@
         <v>49.95</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="84">
       <c r="A17" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="H17" s="13">
         <v>0</v>
@@ -1922,30 +1947,30 @@
         <v>12.99</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="84">
       <c r="A18" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>12</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="H18" s="13">
         <v>0</v>
@@ -1960,30 +1985,30 @@
         <v>15.99</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="98">
       <c r="A19" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G19" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H19" s="13">
         <v>0</v>
@@ -1998,30 +2023,30 @@
         <v>68.75</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="70">
       <c r="A20" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>13</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H20" s="13">
         <v>0</v>
@@ -2036,30 +2061,30 @@
         <v>72.75</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="70">
       <c r="A21" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="H21" s="13">
         <v>0</v>
@@ -2071,33 +2096,33 @@
         <v>99</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="112">
       <c r="A22" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="F22" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="H22" s="13">
         <v>0</v>
@@ -2109,27 +2134,27 @@
         <v>99</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="70">
       <c r="A23" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>157</v>
+        <v>196</v>
       </c>
       <c r="E23" s="15" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>14</v>
@@ -2150,24 +2175,24 @@
         <v>6.99</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="84">
       <c r="A24" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="F24" s="13" t="s">
         <v>14</v>
@@ -2188,30 +2213,30 @@
         <v>4.75</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="70">
       <c r="A25" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>164</v>
+        <v>198</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="H25" s="13">
         <v>0</v>
@@ -2226,30 +2251,30 @@
         <v>12.49</v>
       </c>
       <c r="L25" s="15" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="56">
       <c r="A26" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>166</v>
+        <v>144</v>
       </c>
       <c r="H26" s="13">
         <v>0</v>
@@ -2264,24 +2289,24 @@
         <v>13.49</v>
       </c>
       <c r="L26" s="15" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="70">
       <c r="A27" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="F27" s="13" t="s">
         <v>15</v>
@@ -2302,24 +2327,24 @@
         <v>6.99</v>
       </c>
       <c r="L27" s="15" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="98">
       <c r="A28" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="E28" s="15" t="s">
-        <v>175</v>
+        <v>149</v>
       </c>
       <c r="F28" s="13" t="s">
         <v>15</v>
@@ -2340,7 +2365,7 @@
         <v>199.99</v>
       </c>
       <c r="L28" s="15" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>